<commit_message>
Debut travail sur back_end
</commit_message>
<xml_diff>
--- a/structure.xlsx
+++ b/structure.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>date_modification</t>
+  </si>
+  <si>
+    <t>Account_post_liked</t>
+  </si>
+  <si>
+    <t>commentaire_id_liked</t>
+  </si>
+  <si>
+    <t>post_id_liked</t>
+  </si>
+  <si>
+    <t>Account_commentaire_liked</t>
   </si>
 </sst>
 </file>
@@ -224,6 +236,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -239,14 +259,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,6 +777,148 @@
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
             <a:gd name="adj1" fmla="val -27698"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>986119</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>11205</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Connector 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="986119" y="2924735"/>
+          <a:ext cx="494657" cy="11206"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>966108</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>204109</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Elbow Connector 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="-326571" y="2068286"/>
+          <a:ext cx="3292929" cy="707572"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -28512"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>68036</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Elbow Connector 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="394607" y="1959429"/>
+          <a:ext cx="2789464" cy="503464"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -4634"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1054,17 +1208,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:R23"/>
+  <dimension ref="B3:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
@@ -1083,26 +1236,26 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
-      <c r="K3" s="5" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
+      <c r="K3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="7"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="11"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -1155,16 +1308,16 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="7"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="11"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K8" s="1" t="s">
@@ -1193,16 +1346,16 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="K11" s="5" t="s">
+      <c r="C11" s="8"/>
+      <c r="K11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="5"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -1220,7 +1373,7 @@
       <c r="M12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N12" s="11"/>
+      <c r="N12" s="6"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P14" t="s">
@@ -1228,10 +1381,10 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="8"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -1241,37 +1394,67 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="3" t="s">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="8"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="3"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="2" t="s">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2" t="s">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="9"/>
+      <c r="H29" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="C22:G22"/>
+  <mergeCells count="9">
+    <mergeCell ref="C28:G28"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="K7:R7"/>
     <mergeCell ref="K3:R3"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="K11:M11"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>